<commit_message>
added changes to ddt fail
</commit_message>
<xml_diff>
--- a/jabong/src/test/java/com/qa/testdata/xlstestdata.xlsx
+++ b/jabong/src/test/java/com/qa/testdata/xlstestdata.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>country</t>
   </si>
@@ -91,7 +91,7 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>Please enter last name</t>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -509,7 +509,7 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -538,7 +538,7 @@
         <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
@@ -556,10 +556,10 @@
         <v>20</v>
       </c>
       <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
         <v>24</v>
-      </c>
-      <c r="J3" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>